<commit_message>
Add url of memorial to excel
</commit_message>
<xml_diff>
--- a/ts1.xlsx
+++ b/ts1.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pavel\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Computer\Desktop\BuyingRSREU\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9195"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="53">
   <si>
     <t>RecNo</t>
   </si>
@@ -188,7 +188,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -542,18 +542,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V8"/>
+  <dimension ref="A1:V10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="V4" sqref="V4"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="8.88671875" style="5"/>
+    <col min="1" max="4" width="8.85546875" style="5"/>
+    <col min="5" max="5" width="137.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -621,7 +623,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>134580</v>
       </c>
@@ -663,7 +665,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>134581</v>
       </c>
@@ -707,7 +709,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>134582</v>
       </c>
@@ -753,7 +755,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>134583</v>
       </c>
@@ -797,7 +799,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>134584</v>
       </c>
@@ -841,7 +843,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>134585</v>
       </c>
@@ -885,7 +887,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>134586</v>
       </c>
@@ -929,6 +931,94 @@
         <v>8</v>
       </c>
     </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A9" s="6">
+        <v>134585</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="M9" s="7"/>
+      <c r="N9" s="7"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="7"/>
+      <c r="S9" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="T9" s="7"/>
+      <c r="U9" s="7"/>
+      <c r="V9" s="9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A10" s="6">
+        <v>134586</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="7"/>
+      <c r="R10" s="7"/>
+      <c r="S10" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="T10" s="7"/>
+      <c r="U10" s="7"/>
+      <c r="V10" s="9">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>